<commit_message>
fix: add colon key
</commit_message>
<xml_diff>
--- a/docs/corne-keymap-cheatsheet.xlsx
+++ b/docs/corne-keymap-cheatsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbastian/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbastian/repos/zmk-config/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217208B3-AAE3-0545-9C19-6057E78F6833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE4B99D-222C-1744-BA28-8656003E375F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39520" yWindow="500" windowWidth="29280" windowHeight="26840" xr2:uid="{08513D3C-30BD-D340-9200-D0E4085AEFAF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="118">
   <si>
     <t>Base</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>&amp;lt L1 RET</t>
+  </si>
+  <si>
+    <t>:</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +422,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -465,6 +474,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -784,7 +796,7 @@
   <dimension ref="A3:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,16 +813,16 @@
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -819,16 +831,16 @@
       <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="O5" s="3" t="s">
@@ -839,16 +851,16 @@
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -857,16 +869,16 @@
       <c r="J6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O6" s="4" t="s">
@@ -877,16 +889,16 @@
       <c r="B7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -895,16 +907,16 @@
       <c r="J7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="O7" s="4" t="s">
@@ -941,30 +953,30 @@
       <c r="B15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="3"/>
       <c r="J15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N15" s="3"/>
+      <c r="N15" s="6"/>
       <c r="O15" s="3" t="s">
         <v>113</v>
       </c>
@@ -973,16 +985,16 @@
       <c r="B16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="6" t="s">
         <v>105</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -991,16 +1003,16 @@
       <c r="J16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="N16" s="6"/>
       <c r="O16" s="3" t="s">
         <v>113</v>
       </c>
@@ -1009,24 +1021,24 @@
       <c r="B17" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
         <v>107</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>104</v>
       </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
       <c r="O17" s="3" t="s">
         <v>113</v>
       </c>
@@ -1061,16 +1073,16 @@
       <c r="B24" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -1079,16 +1091,16 @@
       <c r="J24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M24" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="N24" s="6" t="s">
         <v>38</v>
       </c>
       <c r="O24" s="3" t="s">
@@ -1099,16 +1111,16 @@
       <c r="B25" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -1117,16 +1129,16 @@
       <c r="J25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="K25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="L25" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="M25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="N25" s="6" t="s">
         <v>79</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -1137,28 +1149,28 @@
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="3"/>
       <c r="J26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N26" s="6" t="s">
         <v>37</v>
       </c>
       <c r="O26" s="3" t="s">
@@ -1204,32 +1216,32 @@
       <c r="B33" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="6" t="s">
         <v>94</v>
       </c>
       <c r="G33" s="3"/>
       <c r="J33" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="L33" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M33" s="3" t="s">
+      <c r="M33" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="N33" s="3" t="s">
+      <c r="N33" s="6" t="s">
         <v>99</v>
       </c>
       <c r="O33" s="3" t="s">
@@ -1240,32 +1252,32 @@
       <c r="B34" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="6" t="s">
         <v>115</v>
       </c>
       <c r="G34" s="3"/>
       <c r="J34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K34" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="L34" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M34" s="3" t="s">
+      <c r="M34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="N34" s="3" t="s">
+      <c r="N34" s="6" t="s">
         <v>102</v>
       </c>
       <c r="O34" s="3" t="s">
@@ -1276,30 +1288,32 @@
       <c r="B35" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="G35" s="3"/>
       <c r="J35" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K35" s="3" t="s">
+      <c r="K35" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="L35" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="M35" s="3" t="s">
+      <c r="M35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="N35" s="3" t="s">
+      <c r="N35" s="6" t="s">
         <v>103</v>
       </c>
       <c r="O35" s="3" t="s">

</xml_diff>

<commit_message>
feat: change order of volume and brightness func keys
</commit_message>
<xml_diff>
--- a/docs/corne-keymap-cheatsheet.xlsx
+++ b/docs/corne-keymap-cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbastian/repos/zmk-config/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE4B99D-222C-1744-BA28-8656003E375F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAEE7E8-CC03-3142-870D-8C2F04566ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39520" yWindow="500" windowWidth="29280" windowHeight="26840" xr2:uid="{08513D3C-30BD-D340-9200-D0E4085AEFAF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="26840" xr2:uid="{08513D3C-30BD-D340-9200-D0E4085AEFAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -407,6 +407,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -478,6 +486,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA87D852-281C-6D45-81B8-D947A4B5F2F5}">
-  <dimension ref="A3:R37"/>
+  <dimension ref="A3:AF36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,12 +815,12 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:32" ht="27" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -847,7 +858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -885,7 +896,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>82</v>
       </c>
@@ -923,8 +934,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E9" s="3" t="s">
         <v>108</v>
       </c>
@@ -944,400 +955,533 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" ht="27" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="AE13"/>
+      <c r="AF13"/>
+    </row>
+    <row r="14" spans="1:32" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+    </row>
+    <row r="15" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="J15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+    </row>
+    <row r="16" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+    </row>
+    <row r="17" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+    </row>
+    <row r="18" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+    </row>
+    <row r="21" spans="1:32" ht="27" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="3"/>
+      <c r="J25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="R27" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:32" ht="27" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="3"/>
+      <c r="J32" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="K32" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M32" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="N32" s="6"/>
+      <c r="O32" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K33" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="L33" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="M33" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="N33" s="6"/>
+      <c r="O33" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:18" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="3"/>
-      <c r="J26" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="N27" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="R29" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G33" s="3"/>
-      <c r="J33" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="J34" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>102</v>
-      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
       <c r="O34" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="2:15" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="J35" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="O35" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="2:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E37" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L37" s="3" t="s">
+    <row r="35" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L36" s="3" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: updated corne layout cheatsheet
</commit_message>
<xml_diff>
--- a/docs/corne-keymap-cheatsheet.xlsx
+++ b/docs/corne-keymap-cheatsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbastian/repos/zmk-config/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8399233A-B98A-B040-B6D0-D22F282DD258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A73D40A-C9DF-3548-842B-7D80133BD18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11680" yWindow="520" windowWidth="34400" windowHeight="26840" xr2:uid="{08513D3C-30BD-D340-9200-D0E4085AEFAF}"/>
   </bookViews>
@@ -365,18 +365,9 @@
     <t>BT3</t>
   </si>
   <si>
-    <t>LGUI</t>
-  </si>
-  <si>
-    <t>CTRL</t>
-  </si>
-  <si>
     <t>&amp;lt L2 SPC</t>
   </si>
   <si>
-    <t>RALT</t>
-  </si>
-  <si>
     <t>&amp;mo L3</t>
   </si>
   <si>
@@ -393,13 +384,22 @@
   </si>
   <si>
     <t>:</t>
+  </si>
+  <si>
+    <t>&amp;mt CTRL TAB</t>
+  </si>
+  <si>
+    <t>&amp;mt LGUI ESC</t>
+  </si>
+  <si>
+    <t>&amp;mt RALT BS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -431,6 +431,20 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -484,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -511,6 +525,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -833,7 +853,7 @@
   <dimension ref="A3:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,25 +1011,25 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>109</v>
+      <c r="E9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -1055,7 +1075,7 @@
     <row r="14" spans="1:32" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>91</v>
@@ -1088,7 +1108,7 @@
         <v>99</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R14"/>
       <c r="S14"/>
@@ -1109,7 +1129,7 @@
     <row r="15" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>90</v>
@@ -1121,7 +1141,7 @@
         <v>39</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="7"/>
@@ -1142,7 +1162,7 @@
         <v>102</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R15"/>
       <c r="S15"/>
@@ -1163,7 +1183,7 @@
     <row r="16" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>98</v>
@@ -1175,7 +1195,7 @@
         <v>89</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="7"/>
@@ -1196,7 +1216,7 @@
         <v>103</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R16"/>
       <c r="S16"/>
@@ -1252,24 +1272,24 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
@@ -1315,7 +1335,7 @@
     <row r="23" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>65</v>
@@ -1350,13 +1370,13 @@
         <v>38</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>70</v>
@@ -1391,13 +1411,13 @@
         <v>79</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:32" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>75</v>
@@ -1454,30 +1474,30 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="R27" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:32" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -1489,7 +1509,7 @@
     <row r="32" spans="1:32" s="2" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>49</v>
@@ -1518,13 +1538,13 @@
       </c>
       <c r="N32" s="9"/>
       <c r="O32" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>54</v>
@@ -1557,13 +1577,13 @@
       </c>
       <c r="N33" s="9"/>
       <c r="O33" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>81</v>
@@ -1586,7 +1606,7 @@
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
       <c r="O34" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
@@ -1612,24 +1632,24 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>

</xml_diff>

<commit_message>
feat: add RCTRL and RSHFT to the right mods column
</commit_message>
<xml_diff>
--- a/docs/corne-keymap-cheatsheet.xlsx
+++ b/docs/corne-keymap-cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbastian/repos/zmk-config/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A73D40A-C9DF-3548-842B-7D80133BD18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E4E266-0A26-C442-873F-DBC72B819756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11680" yWindow="520" windowWidth="34400" windowHeight="26840" xr2:uid="{08513D3C-30BD-D340-9200-D0E4085AEFAF}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="26840" xr2:uid="{08513D3C-30BD-D340-9200-D0E4085AEFAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>ESC</t>
   </si>
   <si>
-    <t>TAB</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t/>
   </si>
   <si>
-    <t>'</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>RIGHT</t>
   </si>
   <si>
-    <t>DEL</t>
-  </si>
-  <si>
     <t>END</t>
   </si>
   <si>
@@ -287,9 +278,6 @@
     <t>Bright-</t>
   </si>
   <si>
-    <t>&amp;mt LSHIFT / CAPS</t>
-  </si>
-  <si>
     <t>{</t>
   </si>
   <si>
@@ -393,13 +381,25 @@
   </si>
   <si>
     <t>&amp;mt RALT BS</t>
+  </si>
+  <si>
+    <t>&amp;mt LALT TAB</t>
+  </si>
+  <si>
+    <t>&amp;mt LSHIFT CAPS</t>
+  </si>
+  <si>
+    <t>&amp;mt  RCTRL DEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;mt RSHIFT ' </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -445,6 +445,13 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -498,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -515,9 +522,6 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -531,6 +535,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -853,7 +863,7 @@
   <dimension ref="A3:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,173 +877,173 @@
       </c>
     </row>
     <row r="5" spans="1:32" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="5" t="s">
+      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="K6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="M7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="N7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>33</v>
+      <c r="O7" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>115</v>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="L9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+        <v>105</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="12" spans="1:32" ht="27" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1073,42 +1083,42 @@
       <c r="AF13"/>
     </row>
     <row r="14" spans="1:32" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>94</v>
+        <v>106</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>99</v>
+        <v>81</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="R14"/>
       <c r="S14"/>
@@ -1127,42 +1137,42 @@
       <c r="AF14"/>
     </row>
     <row r="15" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>112</v>
+        <v>106</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>102</v>
+        <v>79</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="R15"/>
       <c r="S15"/>
@@ -1181,42 +1191,42 @@
       <c r="AF15"/>
     </row>
     <row r="16" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>114</v>
-      </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="R16"/>
       <c r="S16"/>
@@ -1235,21 +1245,21 @@
       <c r="AF16"/>
     </row>
     <row r="17" spans="1:32" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
       <c r="R17"/>
       <c r="S17"/>
       <c r="T17"/>
@@ -1267,33 +1277,33 @@
       <c r="AF17"/>
     </row>
     <row r="18" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
       <c r="R18"/>
       <c r="S18"/>
       <c r="T18"/>
@@ -1333,171 +1343,171 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:32" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="G23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="E24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="5" t="s">
+      <c r="F24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="K24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="L23" s="9" t="s">
+      <c r="L24" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="M23" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="9" t="s">
+      <c r="M24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="5" t="s">
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="K25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="L24" s="9" t="s">
+      <c r="L25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="M24" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="N24" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="5" t="s">
+      <c r="M25" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="K25" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M25" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="N25" s="9" t="s">
-        <v>37</v>
+      <c r="N25" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:32" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O26" s="7"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O26" s="6"/>
     </row>
     <row r="27" spans="1:32" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
       <c r="R27" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:32" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -1507,153 +1517,153 @@
       </c>
     </row>
     <row r="32" spans="1:32" s="2" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N32" s="8"/>
+      <c r="O32" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L32" s="9" t="s">
+      <c r="F33" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="M32" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="N32" s="9"/>
-      <c r="O32" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K33" s="9" t="s">
+      <c r="M33" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="L33" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M33" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="N33" s="9"/>
+      <c r="N33" s="8"/>
       <c r="O33" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
       <c r="O34" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
     </row>
     <row r="36" spans="1:15" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
       <c r="E36" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
       <c r="J36" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>